<commit_message>
Some Free Syria stuff
</commit_message>
<xml_diff>
--- a/Modding resources/Opinion_modifiers.xlsx
+++ b/Modding resources/Opinion_modifiers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="204">
   <si>
     <t>Key</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>ASEAN Member</t>
+  </si>
+  <si>
+    <t>barbarian_practices</t>
+  </si>
+  <si>
+    <t>Barbaric Practices</t>
   </si>
 </sst>
 </file>
@@ -708,8 +714,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko1" displayName="Taulukko1" ref="B3:H114" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:H114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko1" displayName="Taulukko1" ref="B3:H115" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:H115"/>
   <sortState ref="B4:H114">
     <sortCondition ref="D3:D114"/>
   </sortState>
@@ -989,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H114"/>
+  <dimension ref="B3:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J116" sqref="J116"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>189</v>
       </c>
@@ -2221,12 +2227,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>191</v>
       </c>
       <c r="E114">
         <v>100</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>202</v>
+      </c>
+      <c r="C115" t="s">
+        <v>203</v>
+      </c>
+      <c r="D115">
+        <v>-25</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Syria focus - Pro-Hezbollah branch
</commit_message>
<xml_diff>
--- a/Modding resources/Opinion_modifiers.xlsx
+++ b/Modding resources/Opinion_modifiers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="208">
   <si>
     <t>Key</t>
   </si>
@@ -637,6 +637,12 @@
   </si>
   <si>
     <t>Left Alliance</t>
+  </si>
+  <si>
+    <t>reduced_our_influence</t>
+  </si>
+  <si>
+    <t>Reduced Our Influence</t>
   </si>
 </sst>
 </file>
@@ -720,10 +726,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko1" displayName="Taulukko1" ref="B3:H116" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:H116"/>
-  <sortState ref="B4:H114">
-    <sortCondition ref="D3:D114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko1" displayName="Taulukko1" ref="B3:H117" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:H117"/>
+  <sortState ref="B4:H116">
+    <sortCondition ref="D3:D116"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Key"/>
@@ -1001,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H116"/>
+  <dimension ref="B3:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,65 +1321,71 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="D29">
-        <v>-20</v>
+        <v>-25</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>205</v>
       </c>
       <c r="D30">
-        <v>-20</v>
+        <v>-25</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>165</v>
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
       </c>
       <c r="D31">
         <v>-20</v>
       </c>
-      <c r="G31">
-        <v>12</v>
-      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="D32">
-        <v>-15</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="D33">
-        <v>-15</v>
+        <v>-20</v>
+      </c>
+      <c r="G33">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>-15</v>
@@ -1381,185 +1393,185 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="D35">
         <v>-15</v>
       </c>
-      <c r="G35">
-        <v>36</v>
-      </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>-15</v>
       </c>
-      <c r="G36">
-        <v>50</v>
-      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D37">
-        <v>-10</v>
+        <v>-15</v>
+      </c>
+      <c r="G37">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D38">
-        <v>-10</v>
+        <v>-15</v>
+      </c>
+      <c r="G38">
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D39">
         <v>-10</v>
       </c>
-      <c r="G39">
-        <v>120</v>
-      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D40">
         <v>-10</v>
       </c>
-      <c r="G40">
-        <v>120</v>
-      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <v>-10</v>
       </c>
+      <c r="G41">
+        <v>120</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>98</v>
       </c>
       <c r="D42">
         <v>-10</v>
       </c>
-      <c r="H42">
-        <v>1</v>
+      <c r="G42">
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D43">
-        <v>-5</v>
-      </c>
-      <c r="G43">
-        <v>24</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>-10</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="G45">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="D46">
         <v>5</v>
       </c>
-      <c r="G46">
-        <v>24</v>
-      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>112</v>
       </c>
       <c r="D47">
         <v>5</v>
       </c>
+      <c r="G47">
+        <v>16</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>198</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>114</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
+      <c r="G48">
+        <v>24</v>
+      </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D49">
         <v>5</v>
@@ -1567,29 +1579,32 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>46</v>
+        <v>198</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>199</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>74</v>
+        <v>200</v>
+      </c>
+      <c r="C51" t="s">
+        <v>201</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="D52">
         <v>10</v>
@@ -1597,107 +1612,104 @@
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>133</v>
-      </c>
-      <c r="C53" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="D53">
         <v>10</v>
       </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D54">
         <v>10</v>
       </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="D55">
         <v>10</v>
       </c>
       <c r="G55">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="C56" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="D56">
         <v>10</v>
       </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>54</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="D57">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="G57">
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>195</v>
       </c>
       <c r="D58">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D59">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="D60">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="D61">
         <v>20</v>
@@ -1705,7 +1717,10 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>124</v>
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>20</v>
       </c>
       <c r="D62">
         <v>20</v>
@@ -1713,10 +1728,10 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="D63">
         <v>20</v>
@@ -1724,349 +1739,346 @@
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="D64">
         <v>20</v>
       </c>
-      <c r="G64">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>192</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s">
-        <v>193</v>
+        <v>126</v>
       </c>
       <c r="D65">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>166</v>
+      </c>
+      <c r="D66">
+        <v>20</v>
+      </c>
+      <c r="G66">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" t="s">
+        <v>193</v>
+      </c>
+      <c r="D67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>71</v>
-      </c>
-      <c r="D66">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>73</v>
       </c>
       <c r="D68">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D69">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>81</v>
-      </c>
-      <c r="C70" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D70">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D71">
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D72">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="D73">
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="C74" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="D74">
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D76">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>48</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>49</v>
       </c>
-      <c r="D75">
+      <c r="D77">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>50</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C78" t="s">
         <v>51</v>
       </c>
-      <c r="D76">
+      <c r="D78">
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>151</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>152</v>
       </c>
-      <c r="D77">
+      <c r="D79">
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>94</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>95</v>
-      </c>
-      <c r="D78">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>103</v>
-      </c>
-      <c r="C79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>105</v>
-      </c>
-      <c r="C80" t="s">
-        <v>106</v>
       </c>
       <c r="D80">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D81">
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>106</v>
       </c>
       <c r="D82">
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C83" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="D83">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D84">
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D85">
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>178</v>
+        <v>171</v>
+      </c>
+      <c r="C86" t="s">
+        <v>172</v>
       </c>
       <c r="D86">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="C87" t="s">
+        <v>174</v>
       </c>
       <c r="D87">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D88">
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D89">
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
+        <v>180</v>
+      </c>
+      <c r="D90">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" t="s">
+        <v>182</v>
+      </c>
+      <c r="D91">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>76</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>77</v>
-      </c>
-      <c r="D90">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>78</v>
-      </c>
-      <c r="D91">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>183</v>
-      </c>
-      <c r="C92" t="s">
-        <v>184</v>
       </c>
       <c r="D92">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D93">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" t="s">
+        <v>184</v>
+      </c>
+      <c r="D94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>68</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>69</v>
       </c>
-      <c r="D93">
+      <c r="D95">
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>70</v>
       </c>
-      <c r="D94">
+      <c r="D96">
         <v>200</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" t="s">
-        <v>57</v>
-      </c>
-      <c r="E95">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>58</v>
-      </c>
-      <c r="C96" t="s">
-        <v>59</v>
-      </c>
-      <c r="E96">
-        <v>-25</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E97">
         <v>25</v>
@@ -2074,199 +2086,204 @@
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C98" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E98">
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E99">
-        <v>-25</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C100" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E100">
-        <v>-25</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>75</v>
+        <v>64</v>
+      </c>
+      <c r="C101" t="s">
+        <v>65</v>
       </c>
       <c r="E101">
-        <v>10</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="C102" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="E102">
-        <v>-999</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
       <c r="E103">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C104" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E104">
-        <v>-100</v>
+        <v>-999</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E105">
-        <v>-60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E106">
-        <v>-40</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>159</v>
-      </c>
-      <c r="C107" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E107">
-        <v>-20</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="C108" t="s">
+        <v>158</v>
       </c>
       <c r="E108">
-        <v>-50</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C109" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="E109">
-        <v>50</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E110">
-        <v>20</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C111" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E111">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
+        <v>177</v>
+      </c>
+      <c r="E112">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" t="s">
+        <v>186</v>
+      </c>
+      <c r="E113">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
         <v>187</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C114" t="s">
         <v>188</v>
       </c>
-      <c r="E112">
+      <c r="E114">
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>189</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C115" t="s">
         <v>190</v>
       </c>
-      <c r="E113">
+      <c r="E115">
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>191</v>
       </c>
-      <c r="E114">
+      <c r="E116">
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>202</v>
-      </c>
-      <c r="C115" t="s">
-        <v>203</v>
-      </c>
-      <c r="D115">
-        <v>-25</v>
-      </c>
-      <c r="H115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>204</v>
-      </c>
-      <c r="C116" t="s">
-        <v>205</v>
-      </c>
-      <c r="D116">
-        <v>-25</v>
-      </c>
-      <c r="H116">
-        <v>1</v>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>206</v>
+      </c>
+      <c r="C117" t="s">
+        <v>207</v>
+      </c>
+      <c r="D117">
+        <v>-50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>